<commit_message>
Avance en Ajax y Json
</commit_message>
<xml_diff>
--- a/Modelos_de_Bases_de_Datos/Modelo_Relacional.xlsx
+++ b/Modelos_de_Bases_de_Datos/Modelo_Relacional.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="943" firstSheet="4" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="943" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="REGIONAL" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="177">
   <si>
     <t>Relación REGIONAL</t>
   </si>
@@ -1578,6 +1578,12 @@
   </si>
   <si>
     <t>nombres_usuario</t>
+  </si>
+  <si>
+    <t>Hector Alonso</t>
+  </si>
+  <si>
+    <t>Lopez Valencia</t>
   </si>
 </sst>
 </file>
@@ -1865,6 +1871,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1874,17 +1883,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2274,11 +2280,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
@@ -2317,7 +2323,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8">
@@ -2328,7 +2334,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8">
         <v>17</v>
       </c>
@@ -2337,7 +2343,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8">
         <v>68</v>
       </c>
@@ -2346,7 +2352,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
     </row>
@@ -2376,10 +2382,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="25"/>
     </row>
     <row r="4" spans="1:4" ht="51.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -2409,7 +2415,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -2417,85 +2423,85 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="8"/>
     </row>
     <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="8"/>
     </row>
     <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="25"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:2" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="8"/>
     </row>
     <row r="18" spans="1:2" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:2" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="25"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:2" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="25"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="8"/>
     </row>
     <row r="21" spans="1:2" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="25"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="15"/>
     </row>
     <row r="22" spans="1:2" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="25"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="15"/>
     </row>
     <row r="23" spans="1:2" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="25"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="15"/>
     </row>
     <row r="24" spans="1:2" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="25"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="15"/>
     </row>
     <row r="25" spans="1:2" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="25"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="15"/>
     </row>
   </sheetData>
@@ -2513,7 +2519,7 @@
   <dimension ref="A2:E25"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2527,13 +2533,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="4" spans="1:5" ht="51.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -2587,7 +2593,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="15">
@@ -2604,7 +2610,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="15">
         <v>10</v>
       </c>
@@ -2619,7 +2625,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8">
         <v>25</v>
       </c>
@@ -2634,7 +2640,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8">
         <v>25</v>
       </c>
@@ -2649,7 +2655,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8">
         <v>21</v>
       </c>
@@ -2664,7 +2670,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8">
         <v>21</v>
       </c>
@@ -2679,91 +2685,91 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="8"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="8"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="25"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="8"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="8"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="8"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="8"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="25"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="8"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="25"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="8"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="25"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="25"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="25"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="25"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="25"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -2784,7 +2790,7 @@
   <dimension ref="A2:J12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2800,16 +2806,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="42.75">
       <c r="A4" s="2" t="s">
@@ -2885,7 +2891,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8">
@@ -2911,7 +2917,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8">
         <v>25</v>
       </c>
@@ -2935,7 +2941,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8">
         <v>10</v>
       </c>
@@ -2959,7 +2965,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8">
         <v>21</v>
       </c>
@@ -2983,7 +2989,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8">
         <v>87</v>
       </c>
@@ -3007,7 +3013,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8">
         <v>21</v>
       </c>
@@ -3045,7 +3051,7 @@
   <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3059,13 +3065,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="4" spans="1:7" ht="42.75">
       <c r="A4" s="2" t="s">
@@ -3114,7 +3120,7 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -3131,7 +3137,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8" t="s">
         <v>142</v>
       </c>
@@ -3146,7 +3152,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8" t="s">
         <v>142</v>
       </c>
@@ -3161,21 +3167,21 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -3196,7 +3202,7 @@
   <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3212,15 +3218,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="4" spans="1:9" ht="42.75">
       <c r="A4" s="2" t="s">
@@ -3289,17 +3295,17 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8">
         <v>300</v>
       </c>
       <c r="C7" s="8">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="D7" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E7" s="8">
         <v>21</v>
@@ -3312,7 +3318,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8">
         <v>150</v>
       </c>
@@ -3333,7 +3339,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8">
         <v>500</v>
       </c>
@@ -3354,7 +3360,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -3363,7 +3369,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -3372,7 +3378,7 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -3410,14 +3416,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="4" spans="1:8" ht="51.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -3483,7 +3489,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8">
@@ -3503,7 +3509,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8">
         <v>1135341</v>
       </c>
@@ -3521,7 +3527,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8">
         <v>1320112</v>
       </c>
@@ -3539,7 +3545,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8">
         <v>1135331</v>
       </c>
@@ -3557,7 +3563,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8">
         <v>1124041</v>
       </c>
@@ -3575,7 +3581,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -3583,7 +3589,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -3591,7 +3597,7 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -3622,12 +3628,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="51.75" customHeight="1">
@@ -3674,7 +3680,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8">
@@ -3688,7 +3694,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8">
         <v>223217</v>
       </c>
@@ -3700,7 +3706,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8">
         <v>922717</v>
       </c>
@@ -3712,7 +3718,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8">
         <v>225117</v>
       </c>
@@ -3724,13 +3730,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -3749,8 +3755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3768,18 +3774,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:10" ht="51.75" customHeight="1" thickBot="1">
@@ -3869,7 +3875,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8">
@@ -3893,7 +3899,7 @@
       <c r="H7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="24">
         <v>42846</v>
       </c>
       <c r="J7" s="8">
@@ -3901,7 +3907,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8">
         <v>21</v>
       </c>
@@ -3923,7 +3929,7 @@
       <c r="H8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="24">
         <v>42847</v>
       </c>
       <c r="J8" s="8">
@@ -3931,9 +3937,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>29</v>
@@ -3945,15 +3951,23 @@
         <v>98553377</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+        <v>135</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="I9" s="24">
+        <v>42847</v>
+      </c>
+      <c r="J9" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -3965,7 +3979,7 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -3977,7 +3991,7 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -4021,18 +4035,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:10" ht="51.75" customHeight="1" thickBot="1">
@@ -4122,7 +4136,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8"/>
@@ -4136,7 +4150,7 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -4148,7 +4162,7 @@
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -4160,7 +4174,7 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -4172,7 +4186,7 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -4184,7 +4198,7 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -4227,18 +4241,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:10" ht="51.75" customHeight="1" thickBot="1">
@@ -4328,7 +4342,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8"/>
@@ -4342,7 +4356,7 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -4354,7 +4368,7 @@
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -4366,7 +4380,7 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -4378,7 +4392,7 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -4390,7 +4404,7 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -4428,12 +4442,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="51.75" customHeight="1">
@@ -4480,7 +4494,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8">
@@ -4494,7 +4508,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8">
         <v>9204</v>
       </c>
@@ -4506,7 +4520,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8">
         <v>9206</v>
       </c>
@@ -4518,7 +4532,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8">
         <v>9112</v>
       </c>
@@ -4530,7 +4544,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8">
         <v>9219</v>
       </c>
@@ -4542,7 +4556,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8">
         <v>9220</v>
       </c>
@@ -4554,7 +4568,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="8">
         <v>9309</v>
       </c>
@@ -4566,7 +4580,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="8">
         <v>9224</v>
       </c>
@@ -4578,7 +4592,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="25"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="8">
         <v>9225</v>
       </c>
@@ -4615,12 +4629,12 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" thickBot="1"/>
@@ -4649,7 +4663,7 @@
       <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8"/>
@@ -4657,31 +4671,31 @@
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -4711,10 +4725,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" thickBot="1"/>
@@ -4743,7 +4757,7 @@
       <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8"/>
@@ -4751,31 +4765,31 @@
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -4814,18 +4828,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
     </row>
     <row r="4" spans="1:12" ht="51.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -4916,7 +4930,7 @@
       <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8">
@@ -4954,7 +4968,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8">
         <v>25</v>
       </c>
@@ -4990,7 +5004,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8">
         <v>10</v>
       </c>
@@ -5026,7 +5040,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8">
         <v>21</v>
       </c>
@@ -5062,7 +5076,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8">
         <v>87</v>
       </c>
@@ -5098,7 +5112,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8">
         <v>21</v>
       </c>
@@ -5173,11 +5187,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
@@ -5218,7 +5232,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -5229,7 +5243,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8" t="s">
         <v>29</v>
       </c>
@@ -5238,7 +5252,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8" t="s">
         <v>29</v>
       </c>
@@ -5247,7 +5261,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8" t="s">
         <v>30</v>
       </c>
@@ -5256,7 +5270,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8" t="s">
         <v>30</v>
       </c>
@@ -5265,7 +5279,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
@@ -5274,7 +5288,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="8" t="s">
         <v>31</v>
       </c>
@@ -5296,8 +5310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5313,19 +5327,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="18">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
     </row>
     <row r="4" spans="1:13" ht="51.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -5420,7 +5434,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="21.75" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="15">
@@ -5455,7 +5469,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="15">
         <v>1128387562</v>
       </c>
@@ -5488,7 +5502,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="15">
         <v>70550772</v>
       </c>
@@ -5521,7 +5535,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="15">
         <v>99010212959</v>
       </c>
@@ -5554,7 +5568,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="15">
         <v>70764532</v>
       </c>
@@ -5587,7 +5601,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="15">
         <v>71776164</v>
       </c>
@@ -5620,7 +5634,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="15">
         <v>1017146760</v>
       </c>
@@ -5653,7 +5667,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="15">
         <v>71578068</v>
       </c>
@@ -5686,7 +5700,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="25"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="15">
         <v>99103102304</v>
       </c>
@@ -5719,7 +5733,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="15">
         <v>1020462859</v>
       </c>
@@ -5752,7 +5766,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="15">
         <v>99070611089</v>
       </c>
@@ -5785,7 +5799,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="15">
         <v>1066718643</v>
       </c>
@@ -5818,7 +5832,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="25"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="15">
         <v>1214738471</v>
       </c>
@@ -5851,7 +5865,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="25"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -5864,7 +5878,7 @@
       <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="25"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -5877,7 +5891,7 @@
       <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="25"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -5890,7 +5904,7 @@
       <c r="K22" s="15"/>
     </row>
     <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="25"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -5903,7 +5917,7 @@
       <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="25"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -5945,7 +5959,7 @@
   <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5956,12 +5970,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
     </row>
@@ -6009,7 +6023,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -6023,7 +6037,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="15" t="s">
         <v>93</v>
       </c>
@@ -6035,7 +6049,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="15" t="s">
         <v>93</v>
       </c>
@@ -6047,7 +6061,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="15" t="s">
         <v>93</v>
       </c>
@@ -6059,7 +6073,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="15" t="s">
         <v>93</v>
       </c>
@@ -6071,7 +6085,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="15" t="s">
         <v>93</v>
       </c>
@@ -6083,7 +6097,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -6102,8 +6116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6116,13 +6130,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
@@ -6175,7 +6189,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -6192,7 +6206,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="15" t="s">
         <v>98</v>
       </c>
@@ -6207,7 +6221,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="15" t="s">
         <v>98</v>
       </c>
@@ -6222,7 +6236,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="15" t="s">
         <v>98</v>
       </c>
@@ -6237,7 +6251,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="15" t="s">
         <v>98</v>
       </c>
@@ -6252,7 +6266,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="15" t="s">
         <v>101</v>
       </c>
@@ -6267,7 +6281,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="15" t="s">
         <v>101</v>
       </c>
@@ -6282,21 +6296,21 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="25"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -6317,7 +6331,7 @@
   <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6330,12 +6344,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
     </row>
@@ -6377,7 +6391,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="15">
@@ -6391,7 +6405,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="15">
         <v>20</v>
       </c>
@@ -6403,7 +6417,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="15">
         <v>20</v>
       </c>
@@ -6415,7 +6429,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -6447,13 +6461,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
@@ -6497,7 +6511,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="15">
@@ -6514,7 +6528,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="15">
         <v>675</v>
       </c>
@@ -6529,7 +6543,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="15">
         <v>612</v>
       </c>
@@ -6544,7 +6558,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="15">
         <v>611</v>
       </c>
@@ -6559,28 +6573,28 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="15"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="15"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="15"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -6613,11 +6627,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="18">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
     </row>
     <row r="4" spans="1:5" ht="51.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -6656,7 +6670,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8">
@@ -6667,7 +6681,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8">
         <v>98553377</v>
       </c>
@@ -6676,7 +6690,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="8">
         <v>98553377</v>
       </c>
@@ -6685,7 +6699,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8">
         <v>1128387562</v>
       </c>
@@ -6694,7 +6708,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8">
         <v>70550772</v>
       </c>
@@ -6703,7 +6717,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8">
         <v>70764532</v>
       </c>
@@ -6712,7 +6726,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="8">
         <v>70764532</v>
       </c>
@@ -6721,7 +6735,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="8">
         <v>71776164</v>
       </c>
@@ -6730,7 +6744,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="25"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="8">
         <v>1017146760</v>
       </c>
@@ -6739,7 +6753,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="8">
         <v>1017146760</v>
       </c>
@@ -6748,7 +6762,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="8">
         <v>71578068</v>
       </c>
@@ -6757,7 +6771,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="8">
         <v>71578068</v>
       </c>
@@ -6766,37 +6780,37 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="25"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="8"/>
       <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="25"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="8"/>
       <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="25"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
     </row>
     <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="25"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="25"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="25"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="25"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
     </row>

</xml_diff>